<commit_message>
added a new plot
</commit_message>
<xml_diff>
--- a/p2/packet+rssi-plugins.xlsx
+++ b/p2/packet+rssi-plugins.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binmahi.d\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deema/Desktop/wireless_network/p2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>0m</t>
   </si>
@@ -47,9 +50,6 @@
     <t>4m</t>
   </si>
   <si>
-    <t>d=3.57*squarerootofh</t>
-  </si>
-  <si>
     <t>D=</t>
   </si>
 </sst>
@@ -60,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -247,34 +247,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1139</c:v>
+                  <c:v>1139.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>875</c:v>
+                  <c:v>875.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1081</c:v>
+                  <c:v>1081.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1631</c:v>
+                  <c:v>1631.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1787</c:v>
+                  <c:v>1787.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1465</c:v>
+                  <c:v>1465.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>649</c:v>
+                  <c:v>649.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>766</c:v>
+                  <c:v>766.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1795</c:v>
+                  <c:v>1795.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1459</c:v>
+                  <c:v>1459.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -286,34 +286,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-44.229119123688001</c:v>
+                  <c:v>-44.229119123688</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-43.800192122958997</c:v>
+                  <c:v>-43.800192122959</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-46.304671968191002</c:v>
+                  <c:v>-46.304671968191</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-45.883069427526998</c:v>
+                  <c:v>-45.883069427527</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-42.816894018888</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-44.695890410959002</c:v>
+                  <c:v>-44.695890410959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-41.635748792271002</c:v>
+                  <c:v>-41.635748792271</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-45.140382317802001</c:v>
+                  <c:v>-45.140382317802</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-41.046496815287</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-40.796261682242999</c:v>
+                  <c:v>-40.796261682243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,34 +357,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1056</c:v>
+                  <c:v>1056.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>887</c:v>
+                  <c:v>887.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>380</c:v>
+                  <c:v>380.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>191</c:v>
+                  <c:v>191.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>811</c:v>
+                  <c:v>811.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>363</c:v>
+                  <c:v>363.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>889</c:v>
+                  <c:v>889.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>487</c:v>
+                  <c:v>487.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>305</c:v>
+                  <c:v>305.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>368</c:v>
+                  <c:v>368.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -399,31 +399,31 @@
                   <c:v>-45.166429587482</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-45.730637161388998</c:v>
+                  <c:v>-45.730637161389</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-45.647840531561002</c:v>
+                  <c:v>-45.647840531561</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-39.050830227041999</c:v>
+                  <c:v>-39.050830227042</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-41.970906068163004</c:v>
+                  <c:v>-41.970906068163</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-37.304563492062996</c:v>
+                  <c:v>-37.304563492063</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-35.553459119496999</c:v>
+                  <c:v>-35.553459119497</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-34.390440720050002</c:v>
+                  <c:v>-34.39044072005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-36.150832517140003</c:v>
+                  <c:v>-36.15083251714</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-37.427983539095003</c:v>
+                  <c:v>-37.427983539095</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -467,34 +467,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>185</c:v>
+                  <c:v>185.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>231</c:v>
+                  <c:v>231.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>123</c:v>
+                  <c:v>123.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>167</c:v>
+                  <c:v>167.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>142</c:v>
+                  <c:v>142.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>146</c:v>
+                  <c:v>146.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>210</c:v>
+                  <c:v>210.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>282</c:v>
+                  <c:v>282.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>152</c:v>
+                  <c:v>152.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>94</c:v>
+                  <c:v>94.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,34 +506,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-52.158437730286998</c:v>
+                  <c:v>-52.158437730287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-54.167923235092999</c:v>
+                  <c:v>-54.167923235093</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-55.667005420053997</c:v>
+                  <c:v>-55.667005420054</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-53.02456286428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-52.219391733819002</c:v>
+                  <c:v>-52.219391733819</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-54.976443264764001</c:v>
+                  <c:v>-54.976443264764</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-54.146733111849002</c:v>
+                  <c:v>-54.146733111849</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-50.782555282555002</c:v>
+                  <c:v>-50.782555282555</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-57.110808973487003</c:v>
+                  <c:v>-57.110808973487</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-50.800431499460998</c:v>
+                  <c:v>-50.800431499461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -577,34 +577,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129</c:v>
+                  <c:v>129.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>72.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77</c:v>
+                  <c:v>77.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>197</c:v>
+                  <c:v>197.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>123</c:v>
+                  <c:v>123.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>119</c:v>
+                  <c:v>119.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>118</c:v>
+                  <c:v>118.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,16 +616,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-46.489717223649997</c:v>
+                  <c:v>-46.48971722365</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-47.915422885571999</c:v>
+                  <c:v>-47.915422885572</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-52.468509984638999</c:v>
+                  <c:v>-52.468509984639</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-54.680592991913997</c:v>
+                  <c:v>-54.680592991914</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-57.350630096368</c:v>
@@ -634,16 +634,16 @@
                   <c:v>-51.998760842627</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-48.967168262653999</c:v>
+                  <c:v>-48.967168262654</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-45.67066521265</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-45.247246022032002</c:v>
+                  <c:v>-45.247246022032</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-46.916946308725002</c:v>
+                  <c:v>-46.916946308725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -687,34 +687,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114</c:v>
+                  <c:v>114.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82</c:v>
+                  <c:v>82.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84</c:v>
+                  <c:v>84.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>117</c:v>
+                  <c:v>117.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>123</c:v>
+                  <c:v>123.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>113</c:v>
+                  <c:v>113.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>103</c:v>
+                  <c:v>103.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>93</c:v>
+                  <c:v>93.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,34 +726,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-50.613496932514998</c:v>
+                  <c:v>-50.613496932515</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-49.896209912536001</c:v>
+                  <c:v>-49.896209912536</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-51.383638211381999</c:v>
+                  <c:v>-51.383638211382</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-60.617983367983001</c:v>
+                  <c:v>-60.617983367983</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-50.065321805956003</c:v>
+                  <c:v>-50.065321805956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-54.803760282021003</c:v>
+                  <c:v>-54.803760282021</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-49.804816223067</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-51.297482837529003</c:v>
+                  <c:v>-51.297482837529</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-57.652868554828999</c:v>
+                  <c:v>-57.652868554829</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-49.941383352872002</c:v>
+                  <c:v>-49.941383352872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -761,7 +761,6 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -769,11 +768,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="245714792"/>
-        <c:axId val="245714400"/>
+        <c:axId val="1695714752"/>
+        <c:axId val="1695719184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="245714792"/>
+        <c:axId val="1695714752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,12 +885,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245714400"/>
+        <c:crossAx val="1695719184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245714400"/>
+        <c:axId val="1695719184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1004,7 +1003,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245714792"/>
+        <c:crossAx val="1695714752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1022,10 +1021,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80750995538643577"/>
-          <c:y val="0.12308366520471879"/>
-          <c:w val="0.11047031854653296"/>
-          <c:h val="0.15440546905587699"/>
+          <c:x val="0.826193600641102"/>
+          <c:y val="0.277715329347508"/>
+          <c:w val="0.110470318546533"/>
+          <c:h val="0.154405469055877"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1057,6 +1056,632 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Line</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of sight distance </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>D0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>0.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>D1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>D2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>2.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.04874241767195</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>D3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>3.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6.183421383020891</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>D4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>4.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1729170512"/>
+        <c:axId val="1728387968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1729170512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1728387968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1728387968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Line of sight</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1729170512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1134,6 +1759,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1650,20 +2315,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>366711</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1677,6 +2858,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1982,21 +3193,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="4" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +3218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
         <v>-44.229119123688001</v>
       </c>
@@ -2015,7 +3226,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" s="1">
         <v>-43.800192122958997</v>
       </c>
@@ -2023,7 +3234,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
         <v>-46.304671968191002</v>
       </c>
@@ -2031,7 +3242,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
         <v>-45.883069427526998</v>
       </c>
@@ -2039,7 +3250,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
         <v>-42.816894018888</v>
       </c>
@@ -2047,7 +3258,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
         <v>-44.695890410959002</v>
       </c>
@@ -2055,7 +3266,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" s="1">
         <v>-41.635748792271002</v>
       </c>
@@ -2063,7 +3274,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B9" s="1">
         <v>-45.140382317802001</v>
       </c>
@@ -2071,7 +3282,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B10" s="1">
         <v>-41.046496815287</v>
       </c>
@@ -2079,7 +3290,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B11" s="1">
         <v>-40.796261682242999</v>
       </c>
@@ -2087,21 +3298,21 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <f>3.57*SQRT(0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" s="1">
         <v>-45.166429587482</v>
       </c>
@@ -2109,7 +3320,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B16" s="1">
         <v>-45.730637161388998</v>
       </c>
@@ -2117,7 +3328,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
         <v>-45.647840531561002</v>
       </c>
@@ -2125,7 +3336,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
         <v>-39.050830227041999</v>
       </c>
@@ -2133,7 +3344,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
         <v>-41.970906068163004</v>
       </c>
@@ -2141,7 +3352,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B20" s="1">
         <v>-37.304563492062996</v>
       </c>
@@ -2149,18 +3360,15 @@
         <v>363</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B21" s="1">
         <v>-35.553459119496999</v>
       </c>
       <c r="C21" s="1">
         <v>889</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B22" s="1">
         <v>-34.390440720050002</v>
       </c>
@@ -2168,7 +3376,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B23" s="1">
         <v>-36.150832517140003</v>
       </c>
@@ -2176,7 +3384,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B24" s="1">
         <v>-37.427983539095003</v>
       </c>
@@ -2184,21 +3392,21 @@
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <f>3.57*SQRT(1)</f>
         <v>3.57</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B28" s="1">
         <v>-52.158437730286998</v>
       </c>
@@ -2206,7 +3414,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B29" s="1">
         <v>-54.167923235092999</v>
       </c>
@@ -2214,7 +3422,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B30" s="1">
         <v>-55.667005420053997</v>
       </c>
@@ -2222,7 +3430,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B31" s="1">
         <v>-53.02456286428</v>
       </c>
@@ -2230,7 +3438,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B32" s="1">
         <v>-52.219391733819002</v>
       </c>
@@ -2238,7 +3446,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B33" s="1">
         <v>-54.976443264764001</v>
       </c>
@@ -2246,7 +3454,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B34" s="1">
         <v>-54.146733111849002</v>
       </c>
@@ -2254,7 +3462,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B35" s="1">
         <v>-50.782555282555002</v>
       </c>
@@ -2262,7 +3470,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B36" s="1">
         <v>-57.110808973487003</v>
       </c>
@@ -2270,7 +3478,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B37" s="1">
         <v>-50.800431499460998</v>
       </c>
@@ -2278,21 +3486,21 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38">
         <f>3.57*SQRT(2)</f>
         <v>5.0487424176719493</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B40" s="1">
         <v>-46.489717223649997</v>
       </c>
@@ -2300,7 +3508,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B41" s="1">
         <v>-47.915422885571999</v>
       </c>
@@ -2308,7 +3516,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B42" s="1">
         <v>-52.468509984638999</v>
       </c>
@@ -2316,7 +3524,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B43" s="1">
         <v>-54.680592991913997</v>
       </c>
@@ -2324,7 +3532,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B44" s="1">
         <v>-57.350630096368</v>
       </c>
@@ -2332,7 +3540,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B45" s="1">
         <v>-51.998760842627</v>
       </c>
@@ -2340,7 +3548,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B46" s="1">
         <v>-48.967168262653999</v>
       </c>
@@ -2348,7 +3556,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B47" s="1">
         <v>-45.67066521265</v>
       </c>
@@ -2356,7 +3564,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B48" s="1">
         <v>-45.247246022032002</v>
       </c>
@@ -2364,7 +3572,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B49" s="1">
         <v>-46.916946308725002</v>
       </c>
@@ -2372,21 +3580,21 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50">
         <f>3.57*SQRT(3)</f>
         <v>6.1834213830208915</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B52" s="1">
         <v>-50.613496932514998</v>
       </c>
@@ -2394,7 +3602,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B53" s="1">
         <v>-49.896209912536001</v>
       </c>
@@ -2402,7 +3610,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B54" s="1">
         <v>-51.383638211381999</v>
       </c>
@@ -2410,7 +3618,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B55" s="1">
         <v>-60.617983367983001</v>
       </c>
@@ -2418,7 +3626,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B56" s="1">
         <v>-50.065321805956003</v>
       </c>
@@ -2426,7 +3634,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B57" s="1">
         <v>-54.803760282021003</v>
       </c>
@@ -2434,7 +3642,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B58" s="1">
         <v>-49.804816223067</v>
       </c>
@@ -2442,7 +3650,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B59" s="1">
         <v>-51.297482837529003</v>
       </c>
@@ -2450,7 +3658,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B60" s="1">
         <v>-57.652868554828999</v>
       </c>
@@ -2458,7 +3666,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B61" s="1">
         <v>-49.941383352872002</v>
       </c>
@@ -2466,9 +3674,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B62">
         <f>3.57*SQRT(4)</f>

</xml_diff>